<commit_message>
WIP: Improve images, and practice rounds UX.
</commit_message>
<xml_diff>
--- a/final/practice.xlsx
+++ b/final/practice.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>left_color</t>
   </si>
@@ -29,7 +29,7 @@
     <t>limegreen</t>
   </si>
   <si>
-    <t>both</t>
+    <t>left,right</t>
   </si>
   <si>
     <t>snow</t>
@@ -49,6 +49,9 @@
   <si>
     <t>left</t>
   </si>
+  <si>
+    <t>left,right,</t>
+  </si>
 </sst>
 </file>
 
@@ -57,7 +60,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -69,13 +72,23 @@
       <name val="Helvetica"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Helvetica"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -91,6 +104,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -214,47 +233,56 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -278,6 +306,7 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -294,10 +323,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="404040"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="BFBFBF"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="499BC9"/>
@@ -491,14 +520,15 @@
   <a:objectDefaults>
     <a:spDef>
       <a:spPr>
-        <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
-          <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
-        </a:blipFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst>
           <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
@@ -513,35 +543,29 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
-                <a:srgbClr val="000000">
-                  <a:alpha val="31034"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
             <a:uFillTx/>
             <a:latin typeface="+mn-lt"/>
             <a:ea typeface="+mn-ea"/>
@@ -794,14 +818,20 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="6350" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:srgbClr val="000000">
+              <a:alpha val="50000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1090,7 +1120,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1373,16 +1403,14 @@
   </sheetPr>
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.6" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="19.6016" style="1" customWidth="1"/>
     <col min="2" max="2" width="19.6016" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.6016" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6016" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.1484" style="1" customWidth="1"/>
     <col min="5" max="5" width="19.6016" style="1" customWidth="1"/>
     <col min="6" max="6" width="19.6016" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.6016" style="1" customWidth="1"/>
@@ -1397,7 +1425,7 @@
       <c r="C1" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" t="s" s="4">
         <v>2</v>
       </c>
       <c r="E1" t="s" s="3">
@@ -1407,657 +1435,669 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" s="4">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="5">
+      <c r="B2" t="s" s="6">
         <v>4</v>
       </c>
-      <c r="C2" t="s" s="6">
+      <c r="C2" t="s" s="7">
         <v>4</v>
       </c>
-      <c r="D2" t="s" s="6">
+      <c r="D2" t="s" s="8">
         <v>5</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="9">
         <v>5</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" ht="20.35" customHeight="1">
-      <c r="A3" s="9">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="10">
+      <c r="B3" t="s" s="12">
         <v>4</v>
       </c>
-      <c r="C3" t="s" s="11">
+      <c r="C3" t="s" s="13">
         <v>4</v>
       </c>
-      <c r="D3" t="s" s="11">
+      <c r="D3" t="s" s="14">
         <v>5</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="15">
         <v>5</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" s="9">
+      <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" t="s" s="10">
+      <c r="B4" t="s" s="12">
         <v>4</v>
       </c>
-      <c r="C4" t="s" s="11">
+      <c r="C4" t="s" s="13">
         <v>4</v>
       </c>
-      <c r="D4" t="s" s="11">
+      <c r="D4" t="s" s="14">
         <v>5</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="15">
         <v>5</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
     </row>
     <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" s="9">
+      <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" t="s" s="10">
+      <c r="B5" t="s" s="12">
         <v>4</v>
       </c>
-      <c r="C5" t="s" s="11">
+      <c r="C5" t="s" s="13">
         <v>4</v>
       </c>
-      <c r="D5" t="s" s="11">
+      <c r="D5" t="s" s="14">
         <v>5</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="15">
         <v>5</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
     </row>
     <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" s="9">
+      <c r="A6" s="11">
         <v>5</v>
       </c>
-      <c r="B6" t="s" s="10">
+      <c r="B6" t="s" s="12">
         <v>4</v>
       </c>
-      <c r="C6" t="s" s="11">
+      <c r="C6" t="s" s="13">
         <v>4</v>
       </c>
-      <c r="D6" t="s" s="11">
+      <c r="D6" t="s" s="14">
         <v>5</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="15">
         <v>5</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
     </row>
     <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" s="9">
+      <c r="A7" s="11">
         <v>6</v>
       </c>
-      <c r="B7" t="s" s="10">
+      <c r="B7" t="s" s="12">
         <v>6</v>
       </c>
-      <c r="C7" t="s" s="11">
+      <c r="C7" t="s" s="13">
         <v>7</v>
       </c>
-      <c r="D7" t="s" s="11">
+      <c r="D7" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="15">
         <v>4</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
     </row>
     <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" s="9">
+      <c r="A8" s="11">
         <v>7</v>
       </c>
-      <c r="B8" t="s" s="10">
+      <c r="B8" t="s" s="12">
         <v>6</v>
       </c>
-      <c r="C8" t="s" s="11">
+      <c r="C8" t="s" s="13">
         <v>7</v>
       </c>
-      <c r="D8" t="s" s="11">
+      <c r="D8" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="15">
         <v>4</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
     </row>
     <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" s="9">
+      <c r="A9" s="11">
         <v>8</v>
       </c>
-      <c r="B9" t="s" s="10">
+      <c r="B9" t="s" s="12">
         <v>6</v>
       </c>
-      <c r="C9" t="s" s="11">
+      <c r="C9" t="s" s="13">
         <v>7</v>
       </c>
-      <c r="D9" t="s" s="11">
+      <c r="D9" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="15">
         <v>4</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
     </row>
     <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" s="9">
+      <c r="A10" s="11">
         <v>9</v>
       </c>
-      <c r="B10" t="s" s="10">
+      <c r="B10" t="s" s="12">
         <v>6</v>
       </c>
-      <c r="C10" t="s" s="11">
+      <c r="C10" t="s" s="13">
         <v>7</v>
       </c>
-      <c r="D10" t="s" s="11">
+      <c r="D10" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="15">
         <v>4</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
     </row>
     <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" s="9">
+      <c r="A11" s="11">
         <v>10</v>
       </c>
-      <c r="B11" t="s" s="10">
+      <c r="B11" t="s" s="12">
         <v>6</v>
       </c>
-      <c r="C11" t="s" s="11">
+      <c r="C11" t="s" s="13">
         <v>7</v>
       </c>
-      <c r="D11" t="s" s="11">
+      <c r="D11" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="15">
         <v>4</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
     </row>
     <row r="12" ht="20.35" customHeight="1">
-      <c r="A12" s="9">
+      <c r="A12" s="11">
         <v>11</v>
       </c>
-      <c r="B12" t="s" s="10">
+      <c r="B12" t="s" s="12">
         <v>6</v>
       </c>
-      <c r="C12" t="s" s="11">
+      <c r="C12" t="s" s="13">
         <v>7</v>
       </c>
-      <c r="D12" t="s" s="11">
+      <c r="D12" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="15">
         <v>4</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
     </row>
     <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" s="9">
+      <c r="A13" s="11">
         <v>12</v>
       </c>
-      <c r="B13" t="s" s="10">
+      <c r="B13" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="C13" t="s" s="11">
+      <c r="C13" t="s" s="13">
         <v>7</v>
       </c>
-      <c r="D13" t="s" s="11">
+      <c r="D13" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="15">
         <v>3</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
     </row>
     <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" s="9">
+      <c r="A14" s="11">
         <v>13</v>
       </c>
-      <c r="B14" t="s" s="10">
+      <c r="B14" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="C14" t="s" s="11">
+      <c r="C14" t="s" s="13">
         <v>7</v>
       </c>
-      <c r="D14" t="s" s="11">
+      <c r="D14" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="E14" s="12">
+      <c r="E14" s="15">
         <v>3</v>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
     </row>
     <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="9">
+      <c r="A15" s="11">
         <v>14</v>
       </c>
-      <c r="B15" t="s" s="10">
+      <c r="B15" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="C15" t="s" s="11">
+      <c r="C15" t="s" s="13">
         <v>7</v>
       </c>
-      <c r="D15" t="s" s="11">
+      <c r="D15" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="15">
         <v>3</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
     </row>
     <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" s="9">
+      <c r="A16" s="11">
         <v>15</v>
       </c>
-      <c r="B16" t="s" s="10">
+      <c r="B16" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="C16" t="s" s="11">
+      <c r="C16" t="s" s="13">
         <v>7</v>
       </c>
-      <c r="D16" t="s" s="11">
+      <c r="D16" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="15">
         <v>3</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
     </row>
     <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" s="9">
+      <c r="A17" s="11">
         <v>16</v>
       </c>
-      <c r="B17" t="s" s="10">
+      <c r="B17" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="C17" t="s" s="11">
+      <c r="C17" t="s" s="13">
         <v>7</v>
       </c>
-      <c r="D17" t="s" s="11">
+      <c r="D17" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="15">
         <v>3</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
     </row>
     <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" s="9">
+      <c r="A18" s="11">
         <v>17</v>
       </c>
-      <c r="B18" t="s" s="10">
+      <c r="B18" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="C18" t="s" s="11">
+      <c r="C18" t="s" s="13">
         <v>7</v>
       </c>
-      <c r="D18" t="s" s="11">
+      <c r="D18" t="s" s="14">
         <v>8</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="15">
         <v>3</v>
       </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
     </row>
     <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" s="9">
+      <c r="A19" s="11">
         <v>18</v>
       </c>
-      <c r="B19" t="s" s="10">
+      <c r="B19" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="C19" t="s" s="11">
+      <c r="C19" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="D19" t="s" s="11">
+      <c r="D19" t="s" s="14">
         <v>11</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="15">
         <v>1</v>
       </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
     </row>
     <row r="20" ht="20.35" customHeight="1">
-      <c r="A20" s="9">
+      <c r="A20" s="11">
         <v>19</v>
       </c>
-      <c r="B20" t="s" s="10">
+      <c r="B20" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="C20" t="s" s="11">
+      <c r="C20" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="D20" t="s" s="11">
+      <c r="D20" t="s" s="14">
         <v>11</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="15">
         <v>1</v>
       </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
     </row>
     <row r="21" ht="20.35" customHeight="1">
-      <c r="A21" s="9">
+      <c r="A21" s="11">
         <v>20</v>
       </c>
-      <c r="B21" t="s" s="10">
+      <c r="B21" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="C21" t="s" s="11">
+      <c r="C21" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="D21" t="s" s="11">
+      <c r="D21" t="s" s="14">
         <v>11</v>
       </c>
-      <c r="E21" s="12">
+      <c r="E21" s="15">
         <v>1</v>
       </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
     </row>
     <row r="22" ht="20.35" customHeight="1">
-      <c r="A22" s="9">
+      <c r="A22" s="11">
         <v>21</v>
       </c>
-      <c r="B22" t="s" s="10">
+      <c r="B22" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="C22" t="s" s="11">
+      <c r="C22" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="D22" t="s" s="11">
+      <c r="D22" t="s" s="14">
         <v>11</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="15">
         <v>1</v>
       </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
     </row>
     <row r="23" ht="20.35" customHeight="1">
-      <c r="A23" s="9">
+      <c r="A23" s="11">
         <v>22</v>
       </c>
-      <c r="B23" t="s" s="10">
+      <c r="B23" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="C23" t="s" s="11">
+      <c r="C23" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="D23" t="s" s="11">
+      <c r="D23" t="s" s="14">
         <v>11</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="15">
         <v>1</v>
       </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
     </row>
     <row r="24" ht="20.35" customHeight="1">
-      <c r="A24" s="9">
+      <c r="A24" s="11">
         <v>23</v>
       </c>
-      <c r="B24" t="s" s="10">
+      <c r="B24" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="C24" t="s" s="11">
+      <c r="C24" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="D24" t="s" s="11">
+      <c r="D24" t="s" s="14">
         <v>11</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="15">
         <v>1</v>
       </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
     </row>
     <row r="25" ht="20.35" customHeight="1">
-      <c r="A25" s="9">
+      <c r="A25" s="11">
         <v>24</v>
       </c>
-      <c r="B25" t="s" s="10">
+      <c r="B25" t="s" s="12">
         <v>6</v>
       </c>
-      <c r="C25" t="s" s="11">
+      <c r="C25" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="D25" t="s" s="11">
+      <c r="D25" t="s" s="14">
         <v>11</v>
       </c>
-      <c r="E25" s="12">
+      <c r="E25" s="15">
         <v>2</v>
       </c>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
     </row>
     <row r="26" ht="20.35" customHeight="1">
-      <c r="A26" s="9">
+      <c r="A26" s="11">
         <v>25</v>
       </c>
-      <c r="B26" t="s" s="10">
+      <c r="B26" t="s" s="12">
         <v>6</v>
       </c>
-      <c r="C26" t="s" s="11">
+      <c r="C26" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="D26" t="s" s="11">
+      <c r="D26" t="s" s="14">
         <v>11</v>
       </c>
-      <c r="E26" s="12">
+      <c r="E26" s="15">
         <v>2</v>
       </c>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
     </row>
     <row r="27" ht="20.35" customHeight="1">
-      <c r="A27" s="9">
+      <c r="A27" s="11">
         <v>26</v>
       </c>
-      <c r="B27" t="s" s="10">
+      <c r="B27" t="s" s="12">
         <v>6</v>
       </c>
-      <c r="C27" t="s" s="11">
+      <c r="C27" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="D27" t="s" s="11">
+      <c r="D27" t="s" s="14">
         <v>11</v>
       </c>
-      <c r="E27" s="12">
+      <c r="E27" s="15">
         <v>2</v>
       </c>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
     </row>
     <row r="28" ht="20.35" customHeight="1">
-      <c r="A28" s="9">
+      <c r="A28" s="11">
         <v>27</v>
       </c>
-      <c r="B28" t="s" s="10">
+      <c r="B28" t="s" s="12">
         <v>6</v>
       </c>
-      <c r="C28" t="s" s="11">
+      <c r="C28" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="D28" t="s" s="11">
+      <c r="D28" t="s" s="14">
         <v>11</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28" s="15">
         <v>2</v>
       </c>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
     </row>
     <row r="29" ht="20.35" customHeight="1">
-      <c r="A29" s="9">
+      <c r="A29" s="11">
         <v>28</v>
       </c>
-      <c r="B29" t="s" s="10">
+      <c r="B29" t="s" s="12">
         <v>6</v>
       </c>
-      <c r="C29" t="s" s="11">
+      <c r="C29" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="D29" t="s" s="11">
+      <c r="D29" t="s" s="14">
         <v>11</v>
       </c>
-      <c r="E29" s="12">
+      <c r="E29" s="15">
         <v>2</v>
       </c>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
     </row>
     <row r="30" ht="20.35" customHeight="1">
-      <c r="A30" s="9">
+      <c r="A30" s="11">
         <v>29</v>
       </c>
-      <c r="B30" t="s" s="10">
+      <c r="B30" t="s" s="12">
         <v>6</v>
       </c>
-      <c r="C30" t="s" s="11">
+      <c r="C30" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="D30" t="s" s="11">
+      <c r="D30" t="s" s="14">
         <v>11</v>
       </c>
-      <c r="E30" s="12">
+      <c r="E30" s="15">
         <v>2</v>
       </c>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
     </row>
     <row r="31" ht="20.35" customHeight="1">
-      <c r="A31" s="9">
+      <c r="A31" s="11">
         <v>30</v>
       </c>
-      <c r="B31" t="s" s="10">
+      <c r="B31" t="s" s="12">
         <v>9</v>
       </c>
-      <c r="C31" t="s" s="11">
+      <c r="C31" t="s" s="13">
         <v>9</v>
       </c>
-      <c r="D31" s="13"/>
-      <c r="E31" s="12">
+      <c r="D31" t="s" s="14">
+        <v>12</v>
+      </c>
+      <c r="E31" s="15">
         <v>6</v>
       </c>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
     </row>
     <row r="32" ht="20.35" customHeight="1">
-      <c r="A32" s="9">
+      <c r="A32" s="11">
         <v>31</v>
       </c>
-      <c r="B32" t="s" s="10">
+      <c r="B32" t="s" s="12">
         <v>6</v>
       </c>
-      <c r="C32" t="s" s="11">
+      <c r="C32" t="s" s="13">
         <v>6</v>
       </c>
-      <c r="D32" s="13"/>
-      <c r="E32" s="12">
+      <c r="D32" t="s" s="14">
+        <v>12</v>
+      </c>
+      <c r="E32" s="15">
         <v>6</v>
       </c>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
     </row>
     <row r="33" ht="20.35" customHeight="1">
-      <c r="A33" s="9">
+      <c r="A33" s="11">
         <v>32</v>
       </c>
-      <c r="B33" t="s" s="10">
+      <c r="B33" t="s" s="12">
         <v>10</v>
       </c>
-      <c r="C33" t="s" s="11">
+      <c r="C33" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="12">
+      <c r="D33" t="s" s="14">
+        <v>12</v>
+      </c>
+      <c r="E33" s="15">
         <v>6</v>
       </c>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
     </row>
     <row r="34" ht="20.35" customHeight="1">
-      <c r="A34" s="9">
+      <c r="A34" s="11">
         <v>33</v>
       </c>
-      <c r="B34" t="s" s="10">
+      <c r="B34" t="s" s="12">
         <v>7</v>
       </c>
-      <c r="C34" t="s" s="11">
+      <c r="C34" t="s" s="13">
         <v>7</v>
       </c>
-      <c r="D34" s="13"/>
-      <c r="E34" s="12">
+      <c r="D34" t="s" s="14">
+        <v>12</v>
+      </c>
+      <c r="E34" s="15">
         <v>6</v>
       </c>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
     </row>
     <row r="35" ht="20.35" customHeight="1">
-      <c r="A35" s="9">
+      <c r="A35" s="11">
         <v>34</v>
       </c>
-      <c r="B35" t="s" s="10">
+      <c r="B35" t="s" s="12">
         <v>7</v>
       </c>
-      <c r="C35" t="s" s="11">
+      <c r="C35" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="D35" s="13"/>
-      <c r="E35" s="12">
+      <c r="D35" t="s" s="14">
+        <v>12</v>
+      </c>
+      <c r="E35" s="15">
         <v>6</v>
       </c>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
     </row>
     <row r="36" ht="20.35" customHeight="1">
-      <c r="A36" s="9">
+      <c r="A36" s="11">
         <v>35</v>
       </c>
-      <c r="B36" t="s" s="10">
+      <c r="B36" t="s" s="12">
         <v>10</v>
       </c>
-      <c r="C36" t="s" s="11">
+      <c r="C36" t="s" s="13">
         <v>7</v>
       </c>
-      <c r="D36" s="13"/>
-      <c r="E36" s="12">
+      <c r="D36" t="s" s="14">
+        <v>12</v>
+      </c>
+      <c r="E36" s="15">
         <v>6</v>
       </c>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>